<commit_message>
delete some VCHAIN files because they had file content (company id) that did not match file name
</commit_message>
<xml_diff>
--- a/nlp/data/VCHAINS/5045867108_VCHAINS.xlsx
+++ b/nlp/data/VCHAINS/5045867108_VCHAINS.xlsx
@@ -14,16 +14,16 @@
     <x:definedName name="CriteriaLabels">'Value Chains'!$A$3:$A$4</x:definedName>
     <x:definedName name="CriteriaValues">'Value Chains'!$B$3:$B$4</x:definedName>
     <x:definedName name="ColumnHeader">'Value Chains'!$A$6:$N$6</x:definedName>
-    <x:definedName name="Data">'Value Chains'!$A$7:$N$11</x:definedName>
-    <x:definedName name="DataConfidenceScore">'Value Chains'!$G$7:$G$11</x:definedName>
-    <x:definedName name="DataRevenue">'Value Chains'!$I$7:$I$11</x:definedName>
+    <x:definedName name="Data">'Value Chains'!$A$7:$N$10</x:definedName>
+    <x:definedName name="DataConfidenceScore">'Value Chains'!$G$7:$G$10</x:definedName>
+    <x:definedName name="DataRevenue">'Value Chains'!$I$7:$I$10</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <x:si>
     <x:t>Value Chains</x:t>
   </x:si>
@@ -31,7 +31,7 @@
     <x:t>Company Name</x:t>
   </x:si>
   <x:si>
-    <x:t>Lite-On Technology Corp</x:t>
+    <x:t>Chemours Co</x:t>
   </x:si>
   <x:si>
     <x:t>Company Id</x:t>
@@ -94,37 +94,28 @@
     <x:t>A</x:t>
   </x:si>
   <x:si>
-    <x:t>Roku Inc</x:t>
+    <x:t>Energy Fuels Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Uranium</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pricewaterhousecoopers LLP</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Private</x:t>
   </x:si>
   <x:si>
     <x:t>Supplier</x:t>
   </x:si>
   <x:si>
-    <x:t>Entertainment Production</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cypress Semiconductor Corp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Private</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Semiconductors</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BBB-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Optomec Inc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Electronic Equipment &amp; Parts</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kioxia Holdings Corp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Japan</x:t>
+    <x:t>Business Support Services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DuPont Group Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Commodity Chemicals</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -578,18 +569,18 @@
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
     <x:pageSetUpPr fitToPage="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:N11"/>
+  <x:dimension ref="A1:N10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="15.700625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="26.300625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="26.310625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="7.830625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="12.710625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="23.040625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="26.790625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="25.680625" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="20.190625" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="16.840625000000003" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="21.920625" style="0" customWidth="1"/>
@@ -605,7 +596,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="2">
-        <x:v>44595.9347222222</x:v>
+        <x:v>44598.6590277778</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:14" customFormat="1" ht="32.26" customHeight="1">
@@ -639,7 +630,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="5" t="n">
-        <x:v>4295891508</x:v>
+        <x:v>5045867108</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:14">
@@ -712,7 +703,7 @@
         <x:v>43132</x:v>
       </x:c>
       <x:c r="I7" s="9" t="n">
-        <x:v>1463</x:v>
+        <x:v>1466</x:v>
       </x:c>
       <x:c r="J7" s="5" t="n">
         <x:v>2</x:v>
@@ -732,7 +723,7 @@
     </x:row>
     <x:row r="8" spans="1:14">
       <x:c r="A8" s="5" t="n">
-        <x:v>4297900917</x:v>
+        <x:v>4295862622</x:v>
       </x:c>
       <x:c r="B8" s="5" t="s">
         <x:v>23</x:v>
@@ -741,51 +732,49 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D8" s="5" t="s">
-        <x:v>24</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E8" s="5" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="F8" s="5" t="s">
-        <x:v>25</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="G8" s="7" t="n">
-        <x:v>0.55678434528</x:v>
+        <x:v>0.666094594184154</x:v>
       </x:c>
       <x:c r="H8" s="8">
-        <x:v>43062</x:v>
+        <x:v>44307</x:v>
       </x:c>
       <x:c r="I8" s="9" t="n">
-        <x:v>1533</x:v>
+        <x:v>291</x:v>
       </x:c>
       <x:c r="J8" s="5" t="n">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K8" s="5" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="L8" s="5" t="n">
-        <x:v>1778388000</x:v>
+        <x:v>1658000</x:v>
       </x:c>
       <x:c r="M8" s="5" t="n">
-        <x:v>93</x:v>
-      </x:c>
-      <x:c r="N8" s="5" t="s">
-        <x:v>22</x:v>
-      </x:c>
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="N8" s="5" t="s"/>
     </x:row>
     <x:row r="9" spans="1:14">
       <x:c r="A9" s="5" t="n">
-        <x:v>4295903116</x:v>
+        <x:v>5000017069</x:v>
       </x:c>
       <x:c r="B9" s="5" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C9" s="5" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="C9" s="5" t="s">
+      <x:c r="D9" s="5" t="s">
         <x:v>27</x:v>
-      </x:c>
-      <x:c r="D9" s="5" t="s">
-        <x:v>24</x:v>
       </x:c>
       <x:c r="E9" s="5" t="s">
         <x:v>20</x:v>
@@ -794,55 +783,53 @@
         <x:v>28</x:v>
       </x:c>
       <x:c r="G9" s="7" t="n">
-        <x:v>0.30366456</x:v>
+        <x:v>0.31675424</x:v>
       </x:c>
       <x:c r="H9" s="8">
-        <x:v>41156</x:v>
+        <x:v>43175</x:v>
       </x:c>
       <x:c r="I9" s="9" t="n">
-        <x:v>3439</x:v>
+        <x:v>1423</x:v>
       </x:c>
       <x:c r="J9" s="5" t="n">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="K9" s="5" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="L9" s="5" t="n">
-        <x:v>2205314000</x:v>
+        <x:v>6794563060</x:v>
       </x:c>
       <x:c r="M9" s="5" t="s"/>
-      <x:c r="N9" s="5" t="s">
-        <x:v>29</x:v>
-      </x:c>
+      <x:c r="N9" s="5" t="s"/>
     </x:row>
     <x:row r="10" spans="1:14">
       <x:c r="A10" s="5" t="n">
-        <x:v>4297422171</x:v>
+        <x:v>5037205994</x:v>
       </x:c>
       <x:c r="B10" s="5" t="s">
-        <x:v>30</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C10" s="5" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="D10" s="5" t="s">
         <x:v>27</x:v>
-      </x:c>
-      <x:c r="D10" s="5" t="s">
-        <x:v>24</x:v>
       </x:c>
       <x:c r="E10" s="5" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="F10" s="5" t="s">
-        <x:v>31</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="G10" s="7" t="n">
-        <x:v>0.29733864</x:v>
+        <x:v>0.2955984</x:v>
       </x:c>
       <x:c r="H10" s="8">
-        <x:v>42452</x:v>
+        <x:v>42186</x:v>
       </x:c>
       <x:c r="I10" s="9" t="n">
-        <x:v>2143</x:v>
+        <x:v>2412</x:v>
       </x:c>
       <x:c r="J10" s="5" t="n">
         <x:v>1</x:v>
@@ -850,49 +837,9 @@
       <x:c r="K10" s="5" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="L10" s="5" t="n">
-        <x:v>8007154</x:v>
-      </x:c>
+      <x:c r="L10" s="5" t="s"/>
       <x:c r="M10" s="5" t="s"/>
       <x:c r="N10" s="5" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:14">
-      <x:c r="A11" s="5" t="n">
-        <x:v>5068663189</x:v>
-      </x:c>
-      <x:c r="B11" s="5" t="s">
-        <x:v>32</x:v>
-      </x:c>
-      <x:c r="C11" s="5" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="D11" s="5" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="E11" s="5" t="s">
-        <x:v>33</x:v>
-      </x:c>
-      <x:c r="F11" s="5" t="s">
-        <x:v>28</x:v>
-      </x:c>
-      <x:c r="G11" s="7" t="n">
-        <x:v>0.2897888</x:v>
-      </x:c>
-      <x:c r="H11" s="8">
-        <x:v>43710</x:v>
-      </x:c>
-      <x:c r="I11" s="9" t="n">
-        <x:v>885</x:v>
-      </x:c>
-      <x:c r="J11" s="5" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="K11" s="5" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="L11" s="5" t="s"/>
-      <x:c r="M11" s="5" t="s"/>
-      <x:c r="N11" s="5" t="s"/>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="1">

</xml_diff>